<commit_message>
Updated term search and document summary results
</commit_message>
<xml_diff>
--- a/data/AuditTeamTerms.xlsx
+++ b/data/AuditTeamTerms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\2015-2019 - Master of Data Science\2019-S2 - Capstone Professional Project\Project Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B669A840-C8A6-448C-9978-47D264BDC399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04E419F-B3F6-49A9-9E8F-BC007B5150C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0147254D-B82F-41AA-851D-302436D8DF75}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="191">
   <si>
     <t>Term</t>
   </si>
@@ -590,13 +590,22 @@
     <t>Alternate</t>
   </si>
   <si>
-    <t>Education capital</t>
-  </si>
-  <si>
-    <t>Debt sustainability</t>
-  </si>
-  <si>
-    <t>Courts backlog</t>
+    <t>Education + capital</t>
+  </si>
+  <si>
+    <t>Year 7 + transition</t>
+  </si>
+  <si>
+    <t>Debt + sustainability</t>
+  </si>
+  <si>
+    <t>Courts + backlog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disability funding + school </t>
+  </si>
+  <si>
+    <t>Disability funding + education</t>
   </si>
 </sst>
 </file>
@@ -635,7 +644,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -952,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5132D346-C76E-4FE7-B6E0-A3DCA8D61F76}">
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,156 +1084,171 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>186</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>187</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>40</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>41</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated term search to match word boundaries, alternate terms, and multiple terms in any order. Updated client term spreadsheet with additional alternate terms.
</commit_message>
<xml_diff>
--- a/data/AuditTeamTerms.xlsx
+++ b/data/AuditTeamTerms.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\2015-2019 - Master of Data Science\2019-S2 - Capstone Professional Project\Project Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04E419F-B3F6-49A9-9E8F-BC007B5150C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCC760D-CAAE-4074-95E4-D92251F4D6DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0147254D-B82F-41AA-851D-302436D8DF75}"/>
   </bookViews>
   <sheets>
-    <sheet name="Performance Audit" sheetId="1" r:id="rId1"/>
-    <sheet name="Local Government Audit" sheetId="2" r:id="rId2"/>
-    <sheet name="IT Audit" sheetId="3" r:id="rId3"/>
+    <sheet name="Performance" sheetId="1" r:id="rId1"/>
+    <sheet name="Local Government" sheetId="2" r:id="rId2"/>
+    <sheet name="IT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="207">
   <si>
     <t>Term</t>
   </si>
@@ -164,15 +164,9 @@
     <t>Apprenticeship</t>
   </si>
   <si>
-    <t>apprentice</t>
-  </si>
-  <si>
     <t>Traineeship</t>
   </si>
   <si>
-    <t>trainee</t>
-  </si>
-  <si>
     <t>State records</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>Alexandrina Council</t>
   </si>
   <si>
-    <t>The Barossa Council</t>
-  </si>
-  <si>
     <t>Barunga West Council</t>
   </si>
   <si>
@@ -602,10 +593,67 @@
     <t>Courts + backlog</t>
   </si>
   <si>
-    <t xml:space="preserve">Disability funding + school </t>
-  </si>
-  <si>
     <t>Disability funding + education</t>
+  </si>
+  <si>
+    <t>Disability funding + school</t>
+  </si>
+  <si>
+    <t>Apprentice</t>
+  </si>
+  <si>
+    <t>Trainee</t>
+  </si>
+  <si>
+    <t>Buses</t>
+  </si>
+  <si>
+    <t>Trains</t>
+  </si>
+  <si>
+    <t>Trams</t>
+  </si>
+  <si>
+    <t>Barossa Council</t>
+  </si>
+  <si>
+    <t>Clare and Gilbert Valleys Council</t>
+  </si>
+  <si>
+    <t>Information Communication Technology</t>
+  </si>
+  <si>
+    <t>Information Technology Project</t>
+  </si>
+  <si>
+    <t>Information Communication Technology Project</t>
+  </si>
+  <si>
+    <t>Information Technology Program</t>
+  </si>
+  <si>
+    <t>Information Communication Technology Program</t>
+  </si>
+  <si>
+    <t>Information Technology Infrastructure</t>
+  </si>
+  <si>
+    <t>Information Technology Procurement</t>
+  </si>
+  <si>
+    <t>Information Technology Risk</t>
+  </si>
+  <si>
+    <t>Information Communication Technology Procurement</t>
+  </si>
+  <si>
+    <t>Councils</t>
+  </si>
+  <si>
+    <t>Local road</t>
+  </si>
+  <si>
+    <t>Council rate</t>
   </si>
 </sst>
 </file>
@@ -961,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5132D346-C76E-4FE7-B6E0-A3DCA8D61F76}">
-  <dimension ref="A1:A56"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,162 +1020,175 @@
     <col min="1" max="1" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1144,7 +1205,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -1184,17 +1245,17 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
@@ -1219,37 +1280,37 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1262,7 +1323,7 @@
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="N26:O26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,388 +1336,400 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1666,10 +1739,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEF903D-80BD-45E9-BC1C-33AAFD302A25}">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,294 +1750,324 @@
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated audit team terms
</commit_message>
<xml_diff>
--- a/data/AuditTeamTerms.xlsx
+++ b/data/AuditTeamTerms.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\2015-2019 - Master of Data Science\2019-S2 - Capstone Professional Project\Project Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCC760D-CAAE-4074-95E4-D92251F4D6DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C66B79-254D-4376-9FF3-BE47D0B126C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0147254D-B82F-41AA-851D-302436D8DF75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0147254D-B82F-41AA-851D-302436D8DF75}"/>
   </bookViews>
   <sheets>
-    <sheet name="Performance" sheetId="1" r:id="rId1"/>
+    <sheet name="IT" sheetId="3" r:id="rId1"/>
     <sheet name="Local Government" sheetId="2" r:id="rId2"/>
-    <sheet name="IT" sheetId="3" r:id="rId3"/>
+    <sheet name="Performance" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="208">
   <si>
     <t>Term</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>Council rate</t>
+  </si>
+  <si>
+    <t>Databases</t>
   </si>
 </sst>
 </file>
@@ -1008,20 +1011,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5132D346-C76E-4FE7-B6E0-A3DCA8D61F76}">
-  <dimension ref="A1:B56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEF903D-80BD-45E9-BC1C-33AAFD302A25}">
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1029,288 +1032,318 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>182</v>
+      <c r="A22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>183</v>
+      <c r="A23" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>21</v>
+      <c r="A24" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
+      <c r="A25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>190</v>
+      <c r="A26" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>191</v>
+      <c r="A27" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>192</v>
+      <c r="A28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>26</v>
+      <c r="A29" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
+      <c r="A30" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>28</v>
+      <c r="A31" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>29</v>
+      <c r="A32" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
+      <c r="A33" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>31</v>
+      <c r="A34" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>184</v>
+      <c r="A35" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>32</v>
+      <c r="A36" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>33</v>
+      <c r="A37" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>34</v>
+      <c r="A38" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>35</v>
+      <c r="A39" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>36</v>
+      <c r="A40" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>37</v>
+      <c r="A41" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>38</v>
+      <c r="A42" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>185</v>
+      <c r="A43" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>187</v>
+      <c r="A44" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>186</v>
+      <c r="A45" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>39</v>
+      <c r="A46" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>40</v>
+      <c r="A47" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>41</v>
+      <c r="A48" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>42</v>
+      <c r="A49" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>188</v>
+      <c r="A50" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>43</v>
+      <c r="A51" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>189</v>
+      <c r="A52" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>44</v>
+      <c r="A53" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>45</v>
+      <c r="A54" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>46</v>
+      <c r="A55" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>47</v>
+      <c r="A56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1322,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C504666-6029-40B5-BDE4-615D8FE8D902}">
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1738,20 +1771,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEF903D-80BD-45E9-BC1C-33AAFD302A25}">
-  <dimension ref="A1:B58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5132D346-C76E-4FE7-B6E0-A3DCA8D61F76}">
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1759,315 +1792,288 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" t="s">
-        <v>195</v>
-      </c>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" t="s">
-        <v>196</v>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" t="s">
-        <v>197</v>
+      <c r="A4" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" t="s">
-        <v>198</v>
+      <c r="A5" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" t="s">
-        <v>199</v>
+      <c r="A6" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>125</v>
+      <c r="A7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>126</v>
+      <c r="A8" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>127</v>
+      <c r="A9" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>128</v>
+      <c r="A10" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>129</v>
+      <c r="A11" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>130</v>
+      <c r="A12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>131</v>
+      <c r="A13" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>132</v>
+      <c r="A14" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>133</v>
+      <c r="A15" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>134</v>
+      <c r="A16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>135</v>
+      <c r="A17" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18" t="s">
-        <v>200</v>
+      <c r="A18" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>137</v>
+      <c r="A19" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" t="s">
-        <v>201</v>
+      <c r="A20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21" t="s">
-        <v>203</v>
+      <c r="A21" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" t="s">
-        <v>202</v>
+      <c r="A22" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>141</v>
+      <c r="A23" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>142</v>
+      <c r="A24" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>143</v>
+      <c r="A25" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>144</v>
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>145</v>
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>146</v>
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>147</v>
+      <c r="A29" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>148</v>
+      <c r="A30" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>149</v>
+      <c r="A31" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>150</v>
+      <c r="A32" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>151</v>
+      <c r="A33" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>152</v>
+      <c r="A34" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>153</v>
+      <c r="A35" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>154</v>
+      <c r="A36" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>155</v>
+      <c r="A37" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>156</v>
+      <c r="A38" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>157</v>
+      <c r="A39" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>158</v>
+      <c r="A40" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>159</v>
+      <c r="A41" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>160</v>
+      <c r="A42" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>161</v>
+      <c r="A43" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>162</v>
+      <c r="A44" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>163</v>
+      <c r="A45" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>164</v>
+      <c r="A46" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>165</v>
+      <c r="A47" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>166</v>
+      <c r="A48" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>167</v>
+      <c r="A49" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>168</v>
+      <c r="A50" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>169</v>
+      <c r="A51" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>170</v>
+      <c r="A52" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>171</v>
+      <c r="A53" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>172</v>
+      <c r="A54" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>173</v>
+      <c r="A55" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>176</v>
+      <c r="A56" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>